<commit_message>
Commit initial for frontend and configuration of dockers frontend and backend - Configuration of docker frontend and backend - Configuration of docker compose - Creation of modules for frontend using React framework:   - Home page   - Prestacion page: Where upload the excel to data loading
</commit_message>
<xml_diff>
--- a/backend/resources/examples/INPUT-EXAMPLE.xlsx
+++ b/backend/resources/examples/INPUT-EXAMPLE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\PortableApps\Documents\Projects\sinasuite-dl\backend\resources\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF33D0F9-E23E-4B57-98FE-C5455355CF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E9F81F-188F-406D-A150-3B5189146E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="204">
   <si>
     <t>CAMPOS DEL EXCEL</t>
   </si>
@@ -92,27 +92,6 @@
     <t>ORMA_BENEFIT_SUBTYPES → BEST_CODE</t>
   </si>
   <si>
-    <t>’</t>
-  </si>
-  <si>
-    <t>Codigo Servicio</t>
-  </si>
-  <si>
-    <t>ORMA_SERVICES → SERV_CODE</t>
-  </si>
-  <si>
-    <t>Codigo Centro</t>
-  </si>
-  <si>
-    <t>ORMA_CENTERS → CENT_CODE</t>
-  </si>
-  <si>
-    <t>Codigo Ambito</t>
-  </si>
-  <si>
-    <t>ORMA_AMBITS → AMBI_CODE</t>
-  </si>
-  <si>
     <t>Unidad Medida</t>
   </si>
   <si>
@@ -402,13 +381,274 @@
   </si>
   <si>
     <t>ORMA_BENEFIT_RELATIONS -&gt; CASB_DURATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERP_Servicio -&gt; Descripcion </t>
+  </si>
+  <si>
+    <t>ORMA_CENTERS → CENT_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Servicio</t>
+  </si>
+  <si>
+    <t>ORMA_AMBITS → AMBI_DESCRIPTION_ES</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>rpm</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>ºC</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>mg/dl</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Ud</t>
+  </si>
+  <si>
+    <t>cmH20</t>
+  </si>
+  <si>
+    <t>kg/m2</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>BOT</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>CAJA</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>CJ</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>DÍA</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>GRA</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>HORA</t>
+  </si>
+  <si>
+    <t>JE</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PALET</t>
+  </si>
+  <si>
+    <t>PAQ.</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PQ</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>MINUTOS</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>MILL-UI</t>
+  </si>
+  <si>
+    <t>MUFC</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>UNID</t>
+  </si>
+  <si>
+    <t>aplicac</t>
+  </si>
+  <si>
+    <t>cm2</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>gotas</t>
+  </si>
+  <si>
+    <t>mEq</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>mgmlmin</t>
+  </si>
+  <si>
+    <t>mmol</t>
+  </si>
+  <si>
+    <t>sobre</t>
+  </si>
+  <si>
+    <t>µg</t>
+  </si>
+  <si>
+    <t>DU</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>GRDL</t>
+  </si>
+  <si>
+    <t>GRMM</t>
+  </si>
+  <si>
+    <t>MLKG</t>
+  </si>
+  <si>
+    <t>µL</t>
+  </si>
+  <si>
+    <t>mg/kg</t>
+  </si>
+  <si>
+    <t>ALL CENTERS NON EXTERNAL</t>
+  </si>
+  <si>
+    <t>Si esta vacio, por defecto carga por cada prestacion los centros no externos</t>
+  </si>
+  <si>
+    <t>PD: Para mejorar el rendimiento, se recomienda elegir un centro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +669,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -657,20 +903,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -684,7 +932,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -698,7 +946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -712,7 +960,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -726,7 +974,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -740,7 +988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -748,18 +996,18 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
@@ -768,26 +1016,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>201</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>202</v>
+      </c>
+      <c r="E15" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -798,30 +1049,30 @@
     </row>
     <row r="19" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -839,17 +1090,17 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="56.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
@@ -857,7 +1108,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
@@ -872,19 +1123,19 @@
         <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -897,11 +1148,12 @@
     </row>
   </sheetData>
   <autoFilter ref="B1:J1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A5A8AE0E-0F96-4F72-AED0-C48E1CDAFC81}">
           <x14:formula1>
             <xm:f>'DATOS GENERALES'!$A$2:$A$71</xm:f>
@@ -920,6 +1172,12 @@
           </x14:formula1>
           <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99A0B4F9-75C7-4AFB-A027-E1695990D90E}">
+          <x14:formula1>
+            <xm:f>'DATOS GENERALES'!$D$2:$D$84</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -928,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A99CCAC7-C6B3-4808-86B9-2FB22341CD44}">
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,412 +1197,691 @@
     <col min="1" max="1" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B9" t="s">
         <v>109</v>
       </c>
-      <c r="C2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B10" t="s">
         <v>110</v>
       </c>
-      <c r="C3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
         <v>111</v>
       </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="D13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="B8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="B11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="D18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="D28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="D29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="D30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D31" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="D32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="D33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="D34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="D35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="D36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="D37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="D38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="D39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="D40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="D41" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="D42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="D43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="D44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="D45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="D46" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="D47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="D48" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="D49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="D50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="D51" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="D52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="D54" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="D55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="D56" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="D57" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="D58" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="D59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="D60" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="D61" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="D62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="D63" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="D64" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="D65" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="D66" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="D67" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="D68" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="D69" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="D70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>108</v>
+      <c r="D71" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>